<commit_message>
Update figures and Table 1
Add estimates at three months of age to all figures.

Remove average number of visits per year (during baseline) from Table
1 to avoid confusion. Replace with visits per year during follow-up.
</commit_message>
<xml_diff>
--- a/output/table1.xlsx
+++ b/output/table1.xlsx
@@ -176,15 +176,6 @@
     <t xml:space="preserve">624 (1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Visits per year (median, IQR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (3, 8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (9, 21)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Follow-up in days for overweight/obese (median, IQR)</t>
   </si>
   <si>
@@ -201,6 +192,15 @@
   </si>
   <si>
     <t xml:space="preserve">1,115 (307, 1,825)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visits per year during follow-up (median, IQR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (2, 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (3, 7)</t>
   </si>
 </sst>
 </file>

</xml_diff>